<commit_message>
CUDA, only for dTAd
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyb\OneDrive - mail.nankai.edu.cn\并行计算技术\OPENMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyb\OneDrive - mail.nankai.edu.cn\并行计算技术\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05054212-5795-45E2-83D9-51E61F16DC98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7727DB57-07DC-420A-818E-3F7E470DD8A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="18">
   <si>
     <t>运行时间，单位(s)</t>
   </si>
@@ -77,6 +77,22 @@
   </si>
   <si>
     <t>去创建线程开销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA，仅dtad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cuda</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cuda总</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cuda部分</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -138,7 +154,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -148,11 +164,14 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -19800,30 +19819,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q132"/>
+  <dimension ref="A1:Q186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R144" sqref="R144"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O157" sqref="O157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -20520,21 +20539,21 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="F38" s="3" t="s">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="F38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="J38" s="3" t="s">
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="J38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -21236,21 +21255,21 @@
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="G78" s="3" t="s">
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="G78" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="L78" s="3" t="s">
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="L78" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -22179,26 +22198,26 @@
       <c r="A114" t="s">
         <v>10</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="G115" s="3" t="s">
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="G115" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H115" s="3"/>
-      <c r="I115" s="3"/>
-      <c r="L115" s="3" t="s">
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="L115" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
@@ -23079,20 +23098,633 @@
       </c>
       <c r="Q132" s="2"/>
     </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="G152" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H152" s="4"/>
+      <c r="I152" s="4"/>
+      <c r="L152" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M152" s="4"/>
+      <c r="N152" s="4"/>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>3</v>
+      </c>
+      <c r="B153" t="s">
+        <v>4</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E153" s="1"/>
+      <c r="F153" t="s">
+        <v>3</v>
+      </c>
+      <c r="G153" t="s">
+        <v>4</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J153" s="1"/>
+      <c r="K153" t="s">
+        <v>3</v>
+      </c>
+      <c r="L153" t="s">
+        <v>4</v>
+      </c>
+      <c r="M153" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N153" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O153" s="1"/>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>128</v>
+      </c>
+      <c r="B154">
+        <v>0.14218838</v>
+      </c>
+      <c r="C154">
+        <v>0.70580854999999998</v>
+      </c>
+      <c r="F154">
+        <v>128</v>
+      </c>
+      <c r="G154">
+        <v>676</v>
+      </c>
+      <c r="H154">
+        <v>616</v>
+      </c>
+      <c r="K154">
+        <v>128</v>
+      </c>
+      <c r="L154">
+        <f t="shared" ref="L154:L169" si="14">B154/G154*1000</f>
+        <v>0.21033784023668639</v>
+      </c>
+      <c r="M154">
+        <f>C154/H154*1000</f>
+        <v>1.1457931006493507</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>256</v>
+      </c>
+      <c r="B155">
+        <v>1.36119203</v>
+      </c>
+      <c r="C155">
+        <v>2.9186605999999999</v>
+      </c>
+      <c r="F155">
+        <v>256</v>
+      </c>
+      <c r="G155">
+        <v>1659</v>
+      </c>
+      <c r="H155">
+        <v>2115</v>
+      </c>
+      <c r="K155">
+        <v>256</v>
+      </c>
+      <c r="L155">
+        <f t="shared" si="14"/>
+        <v>0.82048946955997581</v>
+      </c>
+      <c r="M155">
+        <f t="shared" ref="M155:M169" si="15">C155/H155*1000</f>
+        <v>1.3799813711583924</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>384</v>
+      </c>
+      <c r="B156">
+        <v>4.1844674407301401</v>
+      </c>
+      <c r="C156">
+        <v>3.6004505600000001</v>
+      </c>
+      <c r="F156">
+        <v>384</v>
+      </c>
+      <c r="G156">
+        <v>1825</v>
+      </c>
+      <c r="H156">
+        <v>2789</v>
+      </c>
+      <c r="K156">
+        <v>384</v>
+      </c>
+      <c r="L156">
+        <f t="shared" si="14"/>
+        <v>2.2928588716329532</v>
+      </c>
+      <c r="M156">
+        <f t="shared" si="15"/>
+        <v>1.2909467766224454</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>512</v>
+      </c>
+      <c r="B157">
+        <v>12.182143569999999</v>
+      </c>
+      <c r="C157">
+        <v>5.5624348000000001</v>
+      </c>
+      <c r="F157">
+        <v>512</v>
+      </c>
+      <c r="G157">
+        <v>3740</v>
+      </c>
+      <c r="H157">
+        <v>2979</v>
+      </c>
+      <c r="K157">
+        <v>512</v>
+      </c>
+      <c r="L157">
+        <f t="shared" si="14"/>
+        <v>3.2572576390374328</v>
+      </c>
+      <c r="M157">
+        <f t="shared" si="15"/>
+        <v>1.8672154414232967</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>640</v>
+      </c>
+      <c r="B158">
+        <v>25.184467440733901</v>
+      </c>
+      <c r="C158">
+        <v>15.1844674407313</v>
+      </c>
+      <c r="F158">
+        <v>640</v>
+      </c>
+      <c r="G158">
+        <v>5097</v>
+      </c>
+      <c r="H158">
+        <v>5323</v>
+      </c>
+      <c r="K158">
+        <v>640</v>
+      </c>
+      <c r="L158">
+        <f t="shared" si="14"/>
+        <v>4.9410373632987836</v>
+      </c>
+      <c r="M158">
+        <f t="shared" si="15"/>
+        <v>2.8526145858972951</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>768</v>
+      </c>
+      <c r="B159">
+        <v>31.868529219999999</v>
+      </c>
+      <c r="C159">
+        <v>23.498286581999999</v>
+      </c>
+      <c r="F159">
+        <v>768</v>
+      </c>
+      <c r="G159">
+        <v>4414</v>
+      </c>
+      <c r="H159">
+        <v>6751</v>
+      </c>
+      <c r="K159">
+        <v>768</v>
+      </c>
+      <c r="L159">
+        <f t="shared" si="14"/>
+        <v>7.2198752197553242</v>
+      </c>
+      <c r="M159">
+        <f t="shared" si="15"/>
+        <v>3.4807119807435933</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>896</v>
+      </c>
+      <c r="B160">
+        <v>55.184467440734601</v>
+      </c>
+      <c r="C160">
+        <v>43.184467440734203</v>
+      </c>
+      <c r="F160">
+        <v>896</v>
+      </c>
+      <c r="G160">
+        <v>5802</v>
+      </c>
+      <c r="H160">
+        <v>8417</v>
+      </c>
+      <c r="K160">
+        <v>896</v>
+      </c>
+      <c r="L160">
+        <f t="shared" si="14"/>
+        <v>9.5112835988856599</v>
+      </c>
+      <c r="M160">
+        <f t="shared" si="15"/>
+        <v>5.1306246216863727</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1024</v>
+      </c>
+      <c r="B161">
+        <v>138.184467440731</v>
+      </c>
+      <c r="C161">
+        <v>51.184467440733897</v>
+      </c>
+      <c r="F161">
+        <v>1024</v>
+      </c>
+      <c r="G161">
+        <v>10906</v>
+      </c>
+      <c r="H161">
+        <v>8708</v>
+      </c>
+      <c r="K161">
+        <v>1024</v>
+      </c>
+      <c r="L161">
+        <f t="shared" si="14"/>
+        <v>12.670499490255914</v>
+      </c>
+      <c r="M161">
+        <f t="shared" si="15"/>
+        <v>5.8778671842827173</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1152</v>
+      </c>
+      <c r="B162">
+        <v>99.705498199999994</v>
+      </c>
+      <c r="C162">
+        <v>87.560694255000001</v>
+      </c>
+      <c r="F162">
+        <v>1152</v>
+      </c>
+      <c r="G162">
+        <v>6345</v>
+      </c>
+      <c r="H162">
+        <v>11567</v>
+      </c>
+      <c r="K162">
+        <v>1152</v>
+      </c>
+      <c r="L162">
+        <f t="shared" si="14"/>
+        <v>15.714026509062252</v>
+      </c>
+      <c r="M162">
+        <f t="shared" si="15"/>
+        <v>7.569870688596871</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1280</v>
+      </c>
+      <c r="B163">
+        <v>212.67718826999999</v>
+      </c>
+      <c r="C163">
+        <v>70.197168245</v>
+      </c>
+      <c r="F163">
+        <v>1280</v>
+      </c>
+      <c r="G163">
+        <v>10818</v>
+      </c>
+      <c r="H163">
+        <v>7942</v>
+      </c>
+      <c r="K163">
+        <v>1280</v>
+      </c>
+      <c r="L163">
+        <f t="shared" si="14"/>
+        <v>19.659566303383247</v>
+      </c>
+      <c r="M163">
+        <f t="shared" si="15"/>
+        <v>8.8387267999244532</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1408</v>
+      </c>
+      <c r="B164">
+        <v>232.18446744073501</v>
+      </c>
+      <c r="C164">
+        <v>140.4751784</v>
+      </c>
+      <c r="F164">
+        <v>1408</v>
+      </c>
+      <c r="G164">
+        <v>9693</v>
+      </c>
+      <c r="H164">
+        <v>12640</v>
+      </c>
+      <c r="K164">
+        <v>1408</v>
+      </c>
+      <c r="L164">
+        <f t="shared" si="14"/>
+        <v>23.953829303696999</v>
+      </c>
+      <c r="M164">
+        <f t="shared" si="15"/>
+        <v>11.11354259493671</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1536</v>
+      </c>
+      <c r="B165">
+        <v>419.18446744073401</v>
+      </c>
+      <c r="C165">
+        <v>136.63108869999999</v>
+      </c>
+      <c r="F165">
+        <v>1536</v>
+      </c>
+      <c r="G165">
+        <v>14670</v>
+      </c>
+      <c r="H165">
+        <v>10706</v>
+      </c>
+      <c r="K165">
+        <v>1536</v>
+      </c>
+      <c r="L165">
+        <f t="shared" si="14"/>
+        <v>28.574264992551736</v>
+      </c>
+      <c r="M165">
+        <f t="shared" si="15"/>
+        <v>12.762104305996635</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>1664</v>
+      </c>
+      <c r="B166">
+        <v>429.184467440736</v>
+      </c>
+      <c r="C166">
+        <v>190.18446744073401</v>
+      </c>
+      <c r="F166">
+        <v>1664</v>
+      </c>
+      <c r="G166">
+        <v>13141</v>
+      </c>
+      <c r="H166">
+        <v>12805</v>
+      </c>
+      <c r="K166">
+        <v>1664</v>
+      </c>
+      <c r="L166">
+        <f t="shared" si="14"/>
+        <v>32.659954907597296</v>
+      </c>
+      <c r="M166">
+        <f t="shared" si="15"/>
+        <v>14.852359815754316</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1792</v>
+      </c>
+      <c r="B167">
+        <v>638.14885233999996</v>
+      </c>
+      <c r="C167">
+        <v>147.44270319200001</v>
+      </c>
+      <c r="F167">
+        <v>1792</v>
+      </c>
+      <c r="G167">
+        <v>16652</v>
+      </c>
+      <c r="H167">
+        <v>8719</v>
+      </c>
+      <c r="K167">
+        <v>1792</v>
+      </c>
+      <c r="L167">
+        <f t="shared" si="14"/>
+        <v>38.32265507686764</v>
+      </c>
+      <c r="M167">
+        <f t="shared" si="15"/>
+        <v>16.910506158045649</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>1920</v>
+      </c>
+      <c r="B168">
+        <v>994.18446744073503</v>
+      </c>
+      <c r="C168">
+        <v>355.18446744073202</v>
+      </c>
+      <c r="F168">
+        <v>1920</v>
+      </c>
+      <c r="G168">
+        <v>22916</v>
+      </c>
+      <c r="H168">
+        <v>18705</v>
+      </c>
+      <c r="K168">
+        <v>1920</v>
+      </c>
+      <c r="L168">
+        <f t="shared" si="14"/>
+        <v>43.383857018708987</v>
+      </c>
+      <c r="M168">
+        <f t="shared" si="15"/>
+        <v>18.988744583840258</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>2048</v>
+      </c>
+      <c r="B169">
+        <v>1161.4684852</v>
+      </c>
+      <c r="C169">
+        <v>422.53599036000003</v>
+      </c>
+      <c r="F169">
+        <v>2048</v>
+      </c>
+      <c r="G169">
+        <v>23799</v>
+      </c>
+      <c r="H169">
+        <v>19499</v>
+      </c>
+      <c r="K169">
+        <v>2048</v>
+      </c>
+      <c r="L169">
+        <f t="shared" si="14"/>
+        <v>48.803247413756885</v>
+      </c>
+      <c r="M169">
+        <f t="shared" si="15"/>
+        <v>21.669623588901995</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C171" s="2"/>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C172" s="2"/>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C173" s="2"/>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C174" s="2"/>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C175" s="2"/>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C176" s="2"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="2"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="2"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="2"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="2"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="2"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="2"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="2"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="2"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="2"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A151:C151"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="G152:I152"/>
+    <mergeCell ref="L152:N152"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="J38:L38"/>
     <mergeCell ref="B115:D115"/>
     <mergeCell ref="G115:I115"/>
     <mergeCell ref="L115:N115"/>
     <mergeCell ref="B78:D78"/>
     <mergeCell ref="G78:I78"/>
     <mergeCell ref="L78:N78"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="J38:L38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>